<commit_message>
Integracion solapa objetivos y Sigehos con xlsx EfectoresObjetivos
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Detalles PAMI Cápita.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Detalles PAMI Cápita.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\facoep\Estadisticas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="14">
   <si>
     <t>Ajuste Cápita</t>
   </si>
@@ -64,19 +64,22 @@
   <si>
     <t>Emision</t>
   </si>
+  <si>
+    <t>Ajuste debitos por recupero</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,8 +102,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +120,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,18 +156,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -169,22 +185,30 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -466,11 +490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,6 +510,7 @@
     <col min="9" max="9" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -522,7 +547,9 @@
       <c r="K1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="14"/>
+      <c r="L1" s="17" t="s">
+        <v>13</v>
+      </c>
       <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2175,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>44562</v>
       </c>
@@ -2208,6 +2235,429 @@
       </c>
       <c r="K49" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>44589</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="5">
+        <v>28397</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0</v>
+      </c>
+      <c r="F50" s="1">
+        <v>0</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+      <c r="H50" s="1">
+        <v>19097270.989999998</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>44593</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="5">
+        <v>28501</v>
+      </c>
+      <c r="D51" s="1">
+        <v>71513796.760000005</v>
+      </c>
+      <c r="E51" s="1">
+        <v>0</v>
+      </c>
+      <c r="F51" s="1">
+        <v>0</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>44593</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="5">
+        <v>28502</v>
+      </c>
+      <c r="D52" s="1">
+        <v>69142232.890000001</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3945030.08</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2159032.5499999998</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>44593</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="5">
+        <v>9549</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1">
+        <v>-161118.37</v>
+      </c>
+      <c r="K53" s="1">
+        <v>-9250871.3100000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
+        <v>44593</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="5">
+        <v>9553</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1">
+        <v>-192577.8</v>
+      </c>
+      <c r="K54" s="1">
+        <v>-11075121.67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
+        <v>44593</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="5">
+        <v>9551</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>0</v>
+      </c>
+      <c r="I55" s="1">
+        <v>0</v>
+      </c>
+      <c r="J55" s="1">
+        <v>-163734.14000000001</v>
+      </c>
+      <c r="K55" s="1">
+        <v>-6649743.7800000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>44608</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="5">
+        <v>29157</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>0</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>14302759.35</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
+        <v>44622</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="5">
+        <v>29737</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>35676.449999999997</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
+        <v>44622</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="5">
+        <v>29738</v>
+      </c>
+      <c r="D58" s="1">
+        <v>70126125.370000005</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0</v>
+      </c>
+      <c r="I58" s="1">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="11">
+        <v>44622</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="5">
+        <v>29739</v>
+      </c>
+      <c r="D59" s="1">
+        <v>64008089</v>
+      </c>
+      <c r="E59" s="1">
+        <v>3944711</v>
+      </c>
+      <c r="F59" s="1">
+        <v>7467.7</v>
+      </c>
+      <c r="G59" s="1">
+        <v>5786005.3399999999</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0</v>
+      </c>
+      <c r="I59" s="1">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>44622</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="5">
+        <v>10091</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>0</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="J60" s="16">
+        <v>-40618.769999999997</v>
+      </c>
+      <c r="K60" s="16">
+        <v>-1439066.34</v>
+      </c>
+      <c r="L60" s="18">
+        <v>-1312.59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
+        <v>44622</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="5">
+        <v>10095</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="16">
+        <v>-193758.27</v>
+      </c>
+      <c r="K61" s="16">
+        <v>-6054744.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>